<commit_message>
new pilot ep - called cognitive experiment
</commit_message>
<xml_diff>
--- a/detection grids/items index.xlsx
+++ b/detection grids/items index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuval\Desktop\lab\Thesis\Thesis\detection grids\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuval\Desktop\lab\Thesis\yuvalharr.github.io\detection grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78744FA8-2424-4838-8AA6-2E79CA6D3010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BE59BA-D40E-48C4-B055-57249130F7A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" xr2:uid="{F2CCBFE8-C62B-4D40-8ACA-535D47835DC4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="20">
   <si>
     <t>2b</t>
   </si>
@@ -59,18 +59,6 @@
     <t>1c</t>
   </si>
   <si>
-    <t>2a/2b</t>
-  </si>
-  <si>
-    <t>2d/2c</t>
-  </si>
-  <si>
-    <t>2b/3b</t>
-  </si>
-  <si>
-    <t>2c/3c</t>
-  </si>
-  <si>
     <t>4a</t>
   </si>
   <si>
@@ -83,28 +71,28 @@
     <t>3d</t>
   </si>
   <si>
-    <t>*לשים לב. אובייקט גדול</t>
-  </si>
-  <si>
-    <t>3a/2a</t>
-  </si>
-  <si>
-    <t>3d/2d</t>
-  </si>
-  <si>
     <t>2a</t>
   </si>
   <si>
     <t>2d</t>
   </si>
   <si>
-    <t>*בדיוק באמצע</t>
-  </si>
-  <si>
     <t>1a</t>
   </si>
   <si>
     <t>1d</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>demo2</t>
+  </si>
+  <si>
+    <t>2a/3a</t>
+  </si>
+  <si>
+    <t>2d/3d</t>
   </si>
 </sst>
 </file>
@@ -456,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B72885-E96C-44EF-8901-2C7727017F78}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -468,7 +456,7 @@
     <col min="2" max="2" width="5.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -478,8 +466,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -489,8 +480,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -500,8 +494,11 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>4</v>
       </c>
@@ -511,77 +508,86 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>11</v>
       </c>
@@ -591,8 +597,11 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>12</v>
       </c>
@@ -602,118 +611,271 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>32</v>
       </c>

</xml_diff>